<commit_message>
ADD: permisions admin user and profile
</commit_message>
<xml_diff>
--- a/Thesis.xlsx
+++ b/Thesis.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="26">
   <si>
     <t>idt</t>
   </si>
@@ -68,49 +68,28 @@
     <t>1...2.3..4</t>
   </si>
   <si>
-    <t>2024-01-30T01:54:01.298576</t>
+    <t>2024-01-30T04:28:37.638579</t>
   </si>
   <si>
     <t>false</t>
   </si>
   <si>
-    <t>SUBMITTED</t>
+    <t>ACCEPTED_WITH_CONDITIONS</t>
   </si>
   <si>
     <t/>
   </si>
   <si>
-    <t>lv.venta.models.users.Student@6c55487b</t>
-  </si>
-  <si>
-    <t>lv.venta.models.users.AcademicPersonel@586e8b73</t>
-  </si>
-  <si>
-    <t>[lv.venta.models.users.AcademicPersonel@bfb57e8]</t>
-  </si>
-  <si>
-    <t>[lv.venta.models.Comment@732530d8, lv.venta.models.Comment@82cb05]</t>
-  </si>
-  <si>
-    <t>2</t>
-  </si>
-  <si>
-    <t>Pētījums</t>
-  </si>
-  <si>
-    <t>Research</t>
-  </si>
-  <si>
-    <t>lv.venta.models.users.Student@346cf572</t>
-  </si>
-  <si>
-    <t>lv.venta.models.users.AcademicPersonel@bfb57e8</t>
-  </si>
-  <si>
-    <t>[lv.venta.models.users.AcademicPersonel@586e8b73]</t>
-  </si>
-  <si>
-    <t>[]</t>
+    <t>lv.venta.models.users.Student@34c5736d</t>
+  </si>
+  <si>
+    <t>lv.venta.models.users.AcademicPersonel@4c64a167</t>
+  </si>
+  <si>
+    <t>[lv.venta.models.users.AcademicPersonel@1001d154]</t>
+  </si>
+  <si>
+    <t>[lv.venta.models.Comment@1a9accf1, lv.venta.models.Comment@48f3587]</t>
   </si>
 </sst>
 </file>
@@ -155,7 +134,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:M3"/>
+  <dimension ref="A1:M2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -243,47 +222,6 @@
         <v>25</v>
       </c>
     </row>
-    <row r="3">
-      <c r="A3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B3" t="s">
-        <v>27</v>
-      </c>
-      <c r="C3" t="s">
-        <v>28</v>
-      </c>
-      <c r="D3" t="s">
-        <v>28</v>
-      </c>
-      <c r="E3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F3" t="s">
-        <v>18</v>
-      </c>
-      <c r="G3" t="s">
-        <v>19</v>
-      </c>
-      <c r="H3" t="s">
-        <v>20</v>
-      </c>
-      <c r="I3" t="s">
-        <v>21</v>
-      </c>
-      <c r="J3" t="s">
-        <v>29</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
-      </c>
-      <c r="L3" t="s">
-        <v>31</v>
-      </c>
-      <c r="M3" t="s">
-        <v>32</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>